<commit_message>
outbreak location and country cleaning
</commit_message>
<xml_diff>
--- a/src/zika_compilation/czs_misc_checked.xlsx
+++ b/src/zika_compilation/czs_misc_checked.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Zika\priority-pathogens\src\zika_compilation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7768EF5B-B5B3-485C-8264-8551D762D0E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6E7AC03-215C-470E-9EEA-917309C4C14C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4461" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4461" uniqueCount="461">
   <si>
     <t>id</t>
   </si>
@@ -1326,9 +1326,6 @@
   </si>
   <si>
     <t xml:space="preserve">surveillance reports with ns of infected women and nx of CZS cases </t>
-  </si>
-  <si>
-    <t>unsure</t>
   </si>
   <si>
     <t xml:space="preserve">CZS </t>
@@ -1991,10 +1988,10 @@
   <dimension ref="A1:CZ120"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="CF2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="CY22" sqref="CY22"/>
+      <selection pane="bottomRight" activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2321,13 +2318,13 @@
         <v>100</v>
       </c>
       <c r="CX1" s="43" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="CY1" s="2" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="CZ1" s="2" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="2" spans="1:104" x14ac:dyDescent="0.3">
@@ -2642,7 +2639,7 @@
         <v>119</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C4" s="12">
         <v>1236</v>
@@ -2789,7 +2786,7 @@
         <v>116</v>
       </c>
       <c r="CQ4" s="42" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="CR4" s="12" t="s">
         <v>128</v>
@@ -2801,7 +2798,7 @@
         <v>118</v>
       </c>
       <c r="CX4" s="4" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY4" s="3" t="s">
         <v>410</v>
@@ -3292,7 +3289,7 @@
         <v>141</v>
       </c>
       <c r="B8" s="38" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C8" s="38">
         <v>2704</v>
@@ -3442,7 +3439,7 @@
         <v>118</v>
       </c>
       <c r="CX8" s="37" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY8" s="25" t="s">
         <v>410</v>
@@ -3623,7 +3620,7 @@
         <v>149</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C10" s="15">
         <v>2713</v>
@@ -3787,7 +3784,7 @@
         <v>149</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C11" s="15">
         <v>2713</v>
@@ -3951,7 +3948,7 @@
         <v>149</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C12" s="15">
         <v>2713</v>
@@ -4115,7 +4112,7 @@
         <v>149</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C13" s="15">
         <v>2713</v>
@@ -4282,7 +4279,7 @@
         <v>149</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C14" s="15">
         <v>2713</v>
@@ -4446,7 +4443,7 @@
         <v>149</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C15" s="15">
         <v>2713</v>
@@ -4610,7 +4607,7 @@
         <v>149</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C16" s="15">
         <v>2713</v>
@@ -4912,7 +4909,7 @@
         <v>118</v>
       </c>
       <c r="CX17" s="4" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY17" s="4" t="s">
         <v>411</v>
@@ -5386,7 +5383,7 @@
         <v>118</v>
       </c>
       <c r="CX20" s="4" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY20" s="3" t="s">
         <v>410</v>
@@ -5555,7 +5552,7 @@
         <v>175</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C22" s="26">
         <v>21374</v>
@@ -5696,7 +5693,7 @@
         <v>118</v>
       </c>
       <c r="CX22" s="44" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY22" s="26" t="s">
         <v>410</v>
@@ -5845,7 +5842,7 @@
         <v>118</v>
       </c>
       <c r="CX23" s="4" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY23" s="3" t="s">
         <v>410</v>
@@ -6325,7 +6322,7 @@
         <v>118</v>
       </c>
       <c r="CX26" s="4" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY26" s="3" t="s">
         <v>410</v>
@@ -6632,7 +6629,7 @@
         <v>118</v>
       </c>
       <c r="CX28" s="4" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY28" s="3" t="s">
         <v>410</v>
@@ -6793,7 +6790,7 @@
         <v>118</v>
       </c>
       <c r="CX29" s="4" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY29" s="3" t="s">
         <v>410</v>
@@ -6965,7 +6962,7 @@
         <v>211</v>
       </c>
       <c r="B31" s="32" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C31" s="32">
         <v>6241</v>
@@ -6998,7 +6995,7 @@
         <v>123</v>
       </c>
       <c r="S31" s="33">
-        <v>120</v>
+        <v>28</v>
       </c>
       <c r="T31" s="32" t="s">
         <v>106</v>
@@ -7175,7 +7172,7 @@
         <v>211</v>
       </c>
       <c r="B32" s="32" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C32" s="32">
         <v>6241</v>
@@ -7208,7 +7205,7 @@
         <v>123</v>
       </c>
       <c r="S32" s="33">
-        <v>120</v>
+        <v>51</v>
       </c>
       <c r="T32" s="32" t="s">
         <v>106</v>
@@ -7385,7 +7382,7 @@
         <v>211</v>
       </c>
       <c r="B33" s="32" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C33" s="32">
         <v>6241</v>
@@ -7418,7 +7415,7 @@
         <v>123</v>
       </c>
       <c r="S33" s="33">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="T33" s="32" t="s">
         <v>106</v>
@@ -7900,7 +7897,7 @@
         <v>118</v>
       </c>
       <c r="CX35" s="4" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY35" s="3" t="s">
         <v>410</v>
@@ -8061,7 +8058,7 @@
         <v>118</v>
       </c>
       <c r="CX36" s="4" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY36" s="3" t="s">
         <v>410</v>
@@ -8075,7 +8072,7 @@
         <v>224</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C37" s="15">
         <v>6427</v>
@@ -8273,7 +8270,7 @@
         <v>118</v>
       </c>
       <c r="CX37" s="4" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY37" s="3" t="s">
         <v>410</v>
@@ -8287,7 +8284,7 @@
         <v>224</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C38" s="15">
         <v>6427</v>
@@ -8485,7 +8482,7 @@
         <v>118</v>
       </c>
       <c r="CX38" s="4" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY38" s="3" t="s">
         <v>410</v>
@@ -9111,7 +9108,7 @@
         <v>237</v>
       </c>
       <c r="B43" s="32" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C43" s="32">
         <v>6658</v>
@@ -9251,7 +9248,7 @@
         <v>237</v>
       </c>
       <c r="B44" s="32" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C44" s="32">
         <v>6658</v>
@@ -9391,7 +9388,7 @@
         <v>237</v>
       </c>
       <c r="B45" s="32" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C45" s="32">
         <v>6658</v>
@@ -9681,7 +9678,7 @@
         <v>118</v>
       </c>
       <c r="CX46" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY46" s="3" t="s">
         <v>410</v>
@@ -9845,7 +9842,7 @@
         <v>118</v>
       </c>
       <c r="CX47" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY47" s="3" t="s">
         <v>410</v>
@@ -10134,7 +10131,7 @@
         <v>118</v>
       </c>
       <c r="CX49" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY49" s="3" t="s">
         <v>410</v>
@@ -11055,10 +11052,10 @@
         <v>118</v>
       </c>
       <c r="CX55" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY55" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="CZ55" s="3" t="s">
         <v>415</v>
@@ -11207,13 +11204,13 @@
         <v>118</v>
       </c>
       <c r="CX56" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY56" s="3" t="s">
         <v>420</v>
       </c>
       <c r="CZ56" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="57" spans="1:104" x14ac:dyDescent="0.3">
@@ -11359,13 +11356,13 @@
         <v>118</v>
       </c>
       <c r="CX57" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY57" s="3" t="s">
         <v>420</v>
       </c>
       <c r="CZ57" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="58" spans="1:104" x14ac:dyDescent="0.3">
@@ -11511,13 +11508,13 @@
         <v>118</v>
       </c>
       <c r="CX58" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY58" s="3" t="s">
         <v>420</v>
       </c>
       <c r="CZ58" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="59" spans="1:104" x14ac:dyDescent="0.3">
@@ -11663,13 +11660,13 @@
         <v>118</v>
       </c>
       <c r="CX59" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY59" s="3" t="s">
         <v>420</v>
       </c>
       <c r="CZ59" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="60" spans="1:104" x14ac:dyDescent="0.3">
@@ -11818,13 +11815,13 @@
         <v>118</v>
       </c>
       <c r="CX60" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY60" s="3" t="s">
         <v>420</v>
       </c>
       <c r="CZ60" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="61" spans="1:104" x14ac:dyDescent="0.3">
@@ -11970,13 +11967,13 @@
         <v>118</v>
       </c>
       <c r="CX61" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY61" s="3" t="s">
         <v>420</v>
       </c>
       <c r="CZ61" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="62" spans="1:104" x14ac:dyDescent="0.3">
@@ -12122,13 +12119,13 @@
         <v>118</v>
       </c>
       <c r="CX62" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY62" s="3" t="s">
         <v>420</v>
       </c>
       <c r="CZ62" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="63" spans="1:104" x14ac:dyDescent="0.3">
@@ -12274,13 +12271,13 @@
         <v>118</v>
       </c>
       <c r="CX63" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY63" s="3" t="s">
         <v>420</v>
       </c>
       <c r="CZ63" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="64" spans="1:104" x14ac:dyDescent="0.3">
@@ -12426,13 +12423,13 @@
         <v>118</v>
       </c>
       <c r="CX64" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY64" s="3" t="s">
         <v>420</v>
       </c>
       <c r="CZ64" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="65" spans="1:104" x14ac:dyDescent="0.3">
@@ -12578,13 +12575,13 @@
         <v>118</v>
       </c>
       <c r="CX65" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY65" s="3" t="s">
         <v>420</v>
       </c>
       <c r="CZ65" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="66" spans="1:104" x14ac:dyDescent="0.3">
@@ -12730,13 +12727,13 @@
         <v>118</v>
       </c>
       <c r="CX66" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY66" s="3" t="s">
         <v>420</v>
       </c>
       <c r="CZ66" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="67" spans="1:104" x14ac:dyDescent="0.3">
@@ -12882,13 +12879,13 @@
         <v>118</v>
       </c>
       <c r="CX67" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY67" s="3" t="s">
         <v>420</v>
       </c>
       <c r="CZ67" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="68" spans="1:104" x14ac:dyDescent="0.3">
@@ -13037,13 +13034,13 @@
         <v>118</v>
       </c>
       <c r="CX68" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY68" s="3" t="s">
         <v>420</v>
       </c>
       <c r="CZ68" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="69" spans="1:104" x14ac:dyDescent="0.3">
@@ -13192,13 +13189,13 @@
         <v>118</v>
       </c>
       <c r="CX69" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY69" s="3" t="s">
         <v>420</v>
       </c>
       <c r="CZ69" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="70" spans="1:104" x14ac:dyDescent="0.3">
@@ -13344,13 +13341,13 @@
         <v>118</v>
       </c>
       <c r="CX70" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY70" s="3" t="s">
         <v>420</v>
       </c>
       <c r="CZ70" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="71" spans="1:104" x14ac:dyDescent="0.3">
@@ -13496,13 +13493,13 @@
         <v>118</v>
       </c>
       <c r="CX71" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY71" s="3" t="s">
         <v>420</v>
       </c>
       <c r="CZ71" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="72" spans="1:104" x14ac:dyDescent="0.3">
@@ -13648,13 +13645,13 @@
         <v>118</v>
       </c>
       <c r="CX72" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY72" s="3" t="s">
         <v>420</v>
       </c>
       <c r="CZ72" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="73" spans="1:104" x14ac:dyDescent="0.3">
@@ -13803,13 +13800,13 @@
         <v>118</v>
       </c>
       <c r="CX73" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY73" s="3" t="s">
         <v>420</v>
       </c>
       <c r="CZ73" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="74" spans="1:104" x14ac:dyDescent="0.3">
@@ -13955,13 +13952,13 @@
         <v>118</v>
       </c>
       <c r="CX74" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY74" s="3" t="s">
         <v>420</v>
       </c>
       <c r="CZ74" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="75" spans="1:104" x14ac:dyDescent="0.3">
@@ -14107,13 +14104,13 @@
         <v>118</v>
       </c>
       <c r="CX75" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY75" s="3" t="s">
         <v>420</v>
       </c>
       <c r="CZ75" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="76" spans="1:104" x14ac:dyDescent="0.3">
@@ -14259,13 +14256,13 @@
         <v>118</v>
       </c>
       <c r="CX76" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY76" s="3" t="s">
         <v>420</v>
       </c>
       <c r="CZ76" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="77" spans="1:104" x14ac:dyDescent="0.3">
@@ -14411,13 +14408,13 @@
         <v>118</v>
       </c>
       <c r="CX77" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY77" s="3" t="s">
         <v>420</v>
       </c>
       <c r="CZ77" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="78" spans="1:104" x14ac:dyDescent="0.3">
@@ -14563,13 +14560,13 @@
         <v>118</v>
       </c>
       <c r="CX78" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY78" s="3" t="s">
         <v>420</v>
       </c>
       <c r="CZ78" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="79" spans="1:104" x14ac:dyDescent="0.3">
@@ -14715,13 +14712,13 @@
         <v>118</v>
       </c>
       <c r="CX79" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY79" s="3" t="s">
         <v>420</v>
       </c>
       <c r="CZ79" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="80" spans="1:104" x14ac:dyDescent="0.3">
@@ -14867,13 +14864,13 @@
         <v>118</v>
       </c>
       <c r="CX80" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY80" s="3" t="s">
         <v>420</v>
       </c>
       <c r="CZ80" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="81" spans="1:104" x14ac:dyDescent="0.3">
@@ -15019,13 +15016,13 @@
         <v>118</v>
       </c>
       <c r="CX81" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY81" s="3" t="s">
         <v>420</v>
       </c>
       <c r="CZ81" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="82" spans="1:104" x14ac:dyDescent="0.3">
@@ -15171,13 +15168,13 @@
         <v>118</v>
       </c>
       <c r="CX82" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY82" s="3" t="s">
         <v>420</v>
       </c>
       <c r="CZ82" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="83" spans="1:104" x14ac:dyDescent="0.3">
@@ -15323,13 +15320,13 @@
         <v>118</v>
       </c>
       <c r="CX83" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY83" s="3" t="s">
         <v>420</v>
       </c>
       <c r="CZ83" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="84" spans="1:104" x14ac:dyDescent="0.3">
@@ -15475,13 +15472,13 @@
         <v>118</v>
       </c>
       <c r="CX84" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY84" s="3" t="s">
         <v>420</v>
       </c>
       <c r="CZ84" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="85" spans="1:104" x14ac:dyDescent="0.3">
@@ -15627,13 +15624,13 @@
         <v>118</v>
       </c>
       <c r="CX85" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY85" s="3" t="s">
         <v>420</v>
       </c>
       <c r="CZ85" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="86" spans="1:104" x14ac:dyDescent="0.3">
@@ -15779,13 +15776,13 @@
         <v>118</v>
       </c>
       <c r="CX86" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY86" s="3" t="s">
         <v>420</v>
       </c>
       <c r="CZ86" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="87" spans="1:104" x14ac:dyDescent="0.3">
@@ -15931,13 +15928,13 @@
         <v>118</v>
       </c>
       <c r="CX87" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY87" s="3" t="s">
         <v>420</v>
       </c>
       <c r="CZ87" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="88" spans="1:104" x14ac:dyDescent="0.3">
@@ -16086,13 +16083,13 @@
         <v>118</v>
       </c>
       <c r="CX88" s="3" t="s">
-        <v>421</v>
+        <v>459</v>
       </c>
       <c r="CY88" s="3" t="s">
         <v>420</v>
       </c>
       <c r="CZ88" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="89" spans="1:104" x14ac:dyDescent="0.3">
@@ -16393,7 +16390,7 @@
         <v>118</v>
       </c>
       <c r="CX90" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY90" s="3" t="s">
         <v>411</v>
@@ -16741,7 +16738,7 @@
         <v>345</v>
       </c>
       <c r="B93" s="32" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C93" s="32">
         <v>10125</v>
@@ -16867,7 +16864,7 @@
         <v>118</v>
       </c>
       <c r="CX93" s="32" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY93" s="32" t="s">
         <v>410</v>
@@ -17007,13 +17004,13 @@
         <v>118</v>
       </c>
       <c r="CX94" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY94" s="3" t="s">
         <v>410</v>
       </c>
       <c r="CZ94" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="95" spans="1:104" x14ac:dyDescent="0.3">
@@ -17317,7 +17314,7 @@
         <v>118</v>
       </c>
       <c r="CX96" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY96" s="3" t="s">
         <v>419</v>
@@ -17487,7 +17484,7 @@
         <v>118</v>
       </c>
       <c r="CX97" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY97" s="4" t="s">
         <v>411</v>
@@ -17657,7 +17654,7 @@
         <v>118</v>
       </c>
       <c r="CX98" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY98" s="4" t="s">
         <v>411</v>
@@ -18468,7 +18465,7 @@
         <v>116</v>
       </c>
       <c r="CQ103" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="CR103" t="s">
         <v>158</v>
@@ -18494,7 +18491,7 @@
         <v>373</v>
       </c>
       <c r="B104" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C104" s="15">
         <v>11297</v>
@@ -18629,7 +18626,7 @@
         <v>116</v>
       </c>
       <c r="CQ104" s="15" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="CR104" s="15" t="s">
         <v>158</v>
@@ -18655,7 +18652,7 @@
         <v>373</v>
       </c>
       <c r="B105" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C105" s="15">
         <v>11297</v>
@@ -18790,7 +18787,7 @@
         <v>116</v>
       </c>
       <c r="CQ105" s="15" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="CR105" s="15" t="s">
         <v>158</v>
@@ -18816,7 +18813,7 @@
         <v>373</v>
       </c>
       <c r="B106" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C106" s="15">
         <v>11297</v>
@@ -18951,7 +18948,7 @@
         <v>116</v>
       </c>
       <c r="CQ106" s="15" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="CR106" s="15" t="s">
         <v>158</v>
@@ -19551,10 +19548,10 @@
     </row>
     <row r="111" spans="1:104" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B111" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C111" s="15">
         <v>11966</v>
@@ -19698,10 +19695,10 @@
     </row>
     <row r="112" spans="1:104" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B112" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C112" s="15">
         <v>11966</v>
@@ -19845,10 +19842,10 @@
     </row>
     <row r="113" spans="1:104" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B113" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C113" s="15">
         <v>11966</v>
@@ -21075,7 +21072,7 @@
         <v>118</v>
       </c>
       <c r="CX120" s="4" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="CY120" s="4" t="s">
         <v>411</v>

</xml_diff>